<commit_message>
import telegram bot token from file
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E215"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,8 @@
           <t>Cagliari centro</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -493,10 +491,8 @@
           <t>Quadrivano zona San Benedetto/via Machiavelli</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -520,10 +516,8 @@
           <t>Bilocale rifinito</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B4" t="n">
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -547,10 +541,8 @@
           <t>Trasfertisti pressi centro città</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -574,10 +566,8 @@
           <t>Casa 4 studenti ingegneria (via marengo)</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>0</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -601,10 +591,8 @@
           <t>4 LOCALI A CAGLIARI</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="B7" t="n">
+        <v>1000</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -628,10 +616,8 @@
           <t>Appartamento per lavoratori o studenti</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="B8" t="n">
+        <v>1000</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -655,10 +641,8 @@
           <t>Quadrivano cagliari</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="B9" t="n">
+        <v>1000</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -682,10 +666,8 @@
           <t>Bonaria,Rifinitissimo Trivano Arredato Nuovissimo</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B10" t="n">
+        <v>1200</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -709,10 +691,8 @@
           <t>Nuovissimo,ViaDellaPineta x Medici,Docenti,Statali</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B11" t="n">
+        <v>1200</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -736,10 +716,8 @@
           <t>Cagliari, via Fleming luminosa e panoramica casa q</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1350</t>
-        </is>
+      <c r="B12" t="n">
+        <v>1350</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -763,10 +741,8 @@
           <t>Uso transitorio arredato centro Cagliari</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+      <c r="B13" t="n">
+        <v>1500</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -790,10 +766,8 @@
           <t>Posti letto</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>290</t>
-        </is>
+      <c r="B14" t="n">
+        <v>290</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -817,10 +791,8 @@
           <t>Stanza uso Ufficio</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>350</t>
-        </is>
+      <c r="B15" t="n">
+        <v>350</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -844,10 +816,8 @@
           <t>Appartamento zona Piazza Reppubblica</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>520</t>
-        </is>
+      <c r="B16" t="n">
+        <v>520</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -871,10 +841,8 @@
           <t>Piccolo bivano</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
+      <c r="B17" t="n">
+        <v>550</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -898,10 +866,8 @@
           <t>Bivano elegante di 50 mq circa</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>570</t>
-        </is>
+      <c r="B18" t="n">
+        <v>570</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -925,10 +891,8 @@
           <t>Bilocale arredato con terrazza</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>620</t>
-        </is>
+      <c r="B19" t="n">
+        <v>620</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -952,10 +916,8 @@
           <t>Appartamento in centro</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>625</t>
-        </is>
+      <c r="B20" t="n">
+        <v>625</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -979,10 +941,8 @@
           <t>Bivano ristrutturato in centro</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B21" t="n">
+        <v>700</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1006,10 +966,8 @@
           <t>Bivano Corso Vittorio Emanuele</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
+      <c r="B22" t="n">
+        <v>750</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1033,10 +991,8 @@
           <t>P.zza San Benedetto - Trilocale Uso ufficio</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B23" t="n">
+        <v>800</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1060,10 +1016,8 @@
           <t>Signorile Trivano in castello ristrutturato</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B24" t="n">
+        <v>800</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1087,10 +1041,8 @@
           <t>Cagliari bivano TUTTO compreso</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B25" t="n">
+        <v>800</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1114,10 +1066,8 @@
           <t>Quartiere del Sole - trivano con giardino privato</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B26" t="n">
+        <v>800</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1141,10 +1091,8 @@
           <t>Bivano 30 mq Via Carbonia Cagliari</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B27" t="n">
+        <v>800</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1168,10 +1116,8 @@
           <t>Via dante piano alto trivano luminosissimo</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
+      <c r="B28" t="n">
+        <v>850</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1195,10 +1141,8 @@
           <t>Appartamento a Cagliari</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
+      <c r="B29" t="n">
+        <v>850</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1222,10 +1166,8 @@
           <t>Piazza Giovanni XIII - Rifinito bivano arredato</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
+      <c r="B30" t="n">
+        <v>850</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1249,10 +1191,8 @@
           <t>Libera da fine Agosto</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B31" t="n">
+        <v>900</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1276,10 +1216,8 @@
           <t>Monolocale o mansarda</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B32" t="n">
+        <v>0</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1303,10 +1241,8 @@
           <t>Settimanalmente ampio bivano arredato solo due per</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B33" t="n">
+        <v>0</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1330,10 +1266,8 @@
           <t>Intero appartamento o stanze</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B34" t="n">
+        <v>0</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1357,10 +1291,8 @@
           <t>Casa indipendente</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B35" t="n">
+        <v>0</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1384,10 +1316,8 @@
           <t>Persona seria</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B36" t="n">
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1411,10 +1341,8 @@
           <t>Appartamento per lunghi periodi</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B37" t="n">
+        <v>0</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1438,10 +1366,8 @@
           <t>Monolocale/Bilocale</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B38" t="n">
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1465,10 +1391,8 @@
           <t>Mamma con figlio,lavoro a tempo indeterminato</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B39" t="n">
+        <v>0</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1492,10 +1416,8 @@
           <t>Ricerchiamo Appartamenti a Cagliari/hinterland</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B40" t="n">
+        <v>0</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1519,10 +1441,8 @@
           <t>Appartamento per 3 studenti</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B41" t="n">
+        <v>0</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1546,10 +1466,8 @@
           <t>Appartamento in centro</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="B42" t="n">
+        <v>1000</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1573,10 +1491,8 @@
           <t>Appartamento per studenti</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="B43" t="n">
+        <v>1000</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1600,10 +1516,8 @@
           <t>Centralissimo bivano ristrutturato a nuovo</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>1100</t>
-        </is>
+      <c r="B44" t="n">
+        <v>1100</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1627,10 +1541,8 @@
           <t>Cagliari Centro</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B45" t="n">
+        <v>1200</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1654,10 +1566,8 @@
           <t>Giardino per feste</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="B46" t="n">
+        <v>250</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1681,10 +1591,8 @@
           <t>Camere climatizzate zona Sant'avendrace Is Maglias</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+      <c r="B47" t="n">
+        <v>280</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1708,10 +1616,8 @@
           <t>Piccolo appartamento Cagliari hinterland</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+      <c r="B48" t="n">
+        <v>400</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1735,10 +1641,8 @@
           <t>Via Figari -monovano arredato appena ristrutturato</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B49" t="n">
+        <v>500</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1762,10 +1666,8 @@
           <t>Monolocale o bilocale</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B50" t="n">
+        <v>500</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1789,10 +1691,8 @@
           <t>Mono o bilocale</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
+      <c r="B51" t="n">
+        <v>550</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1816,10 +1716,8 @@
           <t>Monolocale zona Piazza Repubblica</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="B52" t="n">
+        <v>650</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1843,10 +1741,8 @@
           <t>Dal 6 Settembre,Bivano Centro 650euro tt compreso</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="B53" t="n">
+        <v>650</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1870,10 +1766,8 @@
           <t>Incantevole appartamento in Castello</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+      <c r="B54" t="n">
+        <v>70</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1897,10 +1791,8 @@
           <t>Via SanGiovanni,Trilocale Arredato x Single Coppie</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B55" t="n">
+        <v>700</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1924,10 +1816,8 @@
           <t>Casa indipendente</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="B56" t="n">
+        <v>80</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1951,10 +1841,8 @@
           <t>Grazioso bivano Cagliari centro</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B57" t="n">
+        <v>800</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1978,10 +1866,8 @@
           <t>Trivano arredato Via della Pineta</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
+      <c r="B58" t="n">
+        <v>850</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2005,10 +1891,8 @@
           <t>Trivano nuovo fronte parco Terramaini</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>898</t>
-        </is>
+      <c r="B59" t="n">
+        <v>898</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2032,10 +1916,8 @@
           <t>Mulinu Becciu, Via Giotto quadrivano</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B60" t="n">
+        <v>900</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2059,10 +1941,8 @@
           <t>Appartamento Cagliari [4/23ARG]</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>950</t>
-        </is>
+      <c r="B61" t="n">
+        <v>950</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2086,10 +1966,8 @@
           <t>Ampio bivano pressi piazza Yenne</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B62" t="n">
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2113,10 +1991,8 @@
           <t>Trasfertisti Cagliari</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B63" t="n">
+        <v>0</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2140,10 +2016,8 @@
           <t>Casa vacanze nel cuore di Cagliari</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B64" t="n">
+        <v>0</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2167,10 +2041,8 @@
           <t>Trivano a Cagliari</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B65" t="n">
+        <v>0</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2194,10 +2066,8 @@
           <t>Delizioso terrazzato attico</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B66" t="n">
+        <v>0</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2221,10 +2091,8 @@
           <t>Piccolo appartamento</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B67" t="n">
+        <v>0</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2248,10 +2116,8 @@
           <t>Bilocale. Zona s.avendrace</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B68" t="n">
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2275,10 +2141,8 @@
           <t>Arborea,appartamento contratto a lungo termine</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B69" t="n">
+        <v>0</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2302,10 +2166,8 @@
           <t>Appartamento SOLO PER IL MESE DI MAGGIO via Tirso</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="B70" t="n">
+        <v>1000</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2329,10 +2191,8 @@
           <t>A 4 studenti fronte facolta' ingegneria</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>1100</t>
-        </is>
+      <c r="B71" t="n">
+        <v>1100</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2356,10 +2216,8 @@
           <t>Luminoso quadrivano Via Figari piano alto</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B72" t="n">
+        <v>1200</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2383,10 +2241,8 @@
           <t>Appartamento bilocale panoramico</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B73" t="n">
+        <v>1200</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2410,10 +2266,8 @@
           <t>Cagliari, via Rockefeller luminosa casa quadrivani</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>1350</t>
-        </is>
+      <c r="B74" t="n">
+        <v>1350</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2437,10 +2291,8 @@
           <t>Attico vista mozzafiato solo referenziati</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>2400</t>
-        </is>
+      <c r="B75" t="n">
+        <v>2400</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2464,10 +2316,8 @@
           <t>Mansarda o stanza</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+      <c r="B76" t="n">
+        <v>300</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2491,10 +2341,8 @@
           <t>Cagliari e hinterland</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B77" t="n">
+        <v>500</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2518,10 +2366,8 @@
           <t>Monolocale non arredato Pirri Via S.Maria Chiara</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B78" t="n">
+        <v>500</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2545,10 +2391,8 @@
           <t>Trivano arredato</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
+      <c r="B79" t="n">
+        <v>550</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2572,10 +2416,8 @@
           <t>Cagliari Castello PICCOLO bivano arredato C/2</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+      <c r="B80" t="n">
+        <v>600</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2599,10 +2441,8 @@
           <t>Cagliari castello piccolo bivano C/2 arredato</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+      <c r="B81" t="n">
+        <v>600</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2626,10 +2466,8 @@
           <t>Grazioso bivano</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B82" t="n">
+        <v>700</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2653,10 +2491,8 @@
           <t>Appartamento a Cagliari - Castello</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B83" t="n">
+        <v>700</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2680,10 +2516,8 @@
           <t>Trilocale ammobiliato</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B84" t="n">
+        <v>700</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2707,10 +2541,8 @@
           <t>Appartamento per lavoratori/ici stagionali</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
+      <c r="B85" t="n">
+        <v>750</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2734,10 +2566,8 @@
           <t>Trilocale in zona Parco Terramaini Pirri</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B86" t="n">
+        <v>800</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2761,10 +2591,8 @@
           <t>SANTA GILLA: BIVANI, mai abitati con balcone</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B87" t="n">
+        <v>800</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2788,10 +2616,8 @@
           <t>Cagliari, Via della Pineta/Via dei Colombi</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B88" t="n">
+        <v>800</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2815,10 +2641,8 @@
           <t>Cagliari La vega quadrivano arredato 2 bagni</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B89" t="n">
+        <v>800</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2842,10 +2666,8 @@
           <t>Trilocale luminoso Monreale con posto auto</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B90" t="n">
+        <v>900</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2869,10 +2691,8 @@
           <t>Appartamento in centro (piazza del Carmine)</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>950</t>
-        </is>
+      <c r="B91" t="n">
+        <v>950</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2896,10 +2716,8 @@
           <t>Appartamento da affittare a Cagliari</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B92" t="n">
+        <v>0</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2923,10 +2741,8 @@
           <t>Studenti per unità abitativa</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B93" t="n">
+        <v>0</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2950,10 +2766,8 @@
           <t>Casa per trasfertisti</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B94" t="n">
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2977,10 +2791,8 @@
           <t>Bilocale Quartiere Villanova</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B95" t="n">
+        <v>0</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -3004,10 +2816,8 @@
           <t>A Piloti/Ass.ti di volo /trasfertisti.Appartamento</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B96" t="n">
+        <v>0</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -3031,10 +2841,8 @@
           <t>Bivani in centro città</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B97" t="n">
+        <v>0</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -3058,10 +2866,8 @@
           <t>Via tola ampio esavano</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B98" t="n">
+        <v>0</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -3085,10 +2891,8 @@
           <t>Stanza studenti</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B99" t="n">
+        <v>0</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -3112,10 +2916,8 @@
           <t>C.e.r.c.a.s.i. appartamento</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B100" t="n">
+        <v>0</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -3139,10 +2941,8 @@
           <t>Appartamento di lusso a Cagliari</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B101" t="n">
+        <v>1200</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -3166,10 +2966,8 @@
           <t>Appartamento signorile</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>1800</t>
-        </is>
+      <c r="B102" t="n">
+        <v>1800</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -3193,10 +2991,8 @@
           <t>Perbrevi e lunghi periodi</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>195</t>
-        </is>
+      <c r="B103" t="n">
+        <v>195</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -3220,10 +3016,8 @@
           <t>Pressi viale Trento monolocale miniappartamento</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+      <c r="B104" t="n">
+        <v>300</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -3247,10 +3041,8 @@
           <t>Stanze all inclusive per studenti internazionali</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+      <c r="B105" t="n">
+        <v>300</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -3274,10 +3066,8 @@
           <t>Luxury panoramic suite in Cagliari</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
+      <c r="B106" t="n">
+        <v>5000</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -3301,10 +3091,8 @@
           <t>Monolocale nuovo</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+      <c r="B107" t="n">
+        <v>600</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -3328,10 +3116,8 @@
           <t>Viale Merello ultimo piano</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="B108" t="n">
+        <v>650</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -3355,10 +3141,8 @@
           <t>Bilocale, arredato, con vista</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+      <c r="B109" t="n">
+        <v>70</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -3382,10 +3166,8 @@
           <t>Grazioso bivano</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B110" t="n">
+        <v>700</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -3409,10 +3191,8 @@
           <t>2 camere, ampio soggiorno, angolo cottura</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B111" t="n">
+        <v>700</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -3436,10 +3216,8 @@
           <t>Bilocale panoramico nuovo</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B112" t="n">
+        <v>700</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -3463,10 +3241,8 @@
           <t>Appartamento in condivisione</t>
         </is>
       </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B113" t="n">
+        <v>700</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -3490,10 +3266,8 @@
           <t>Bilocale Sant Avendrace -via is maglias</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
+      <c r="B114" t="n">
+        <v>750</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -3517,10 +3291,8 @@
           <t>Trilocale zona via Cadello</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
+      <c r="B115" t="n">
+        <v>750</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -3544,10 +3316,8 @@
           <t>Trivano genneruxi</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
+      <c r="B116" t="n">
+        <v>750</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -3571,10 +3341,8 @@
           <t>Cagliari adiacente piazza Yenne trivano arredato</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B117" t="n">
+        <v>800</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -3598,10 +3366,8 @@
           <t>2 LOCALI A CAGLIARI</t>
         </is>
       </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B118" t="n">
+        <v>800</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -3625,10 +3391,8 @@
           <t>Bilocale appena ristrutturato</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B119" t="n">
+        <v>800</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -3652,10 +3416,8 @@
           <t>Quadrivano zona Vesalio</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B120" t="n">
+        <v>900</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -3679,10 +3441,8 @@
           <t>Quadrivano Luminoso Cagliari</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>950</t>
-        </is>
+      <c r="B121" t="n">
+        <v>950</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -3706,10 +3466,8 @@
           <t>Appartamento mesi invernali</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B122" t="n">
+        <v>0</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -3733,10 +3491,8 @@
           <t>Cagliari Quartiere Del Sole Trivano ristrutturato</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B123" t="n">
+        <v>0</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3760,10 +3516,8 @@
           <t>Apparta</t>
         </is>
       </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B124" t="n">
+        <v>0</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3787,10 +3541,8 @@
           <t>Monolocale a soli 3min a piedi da piazza jenne</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B125" t="n">
+        <v>0</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -3814,10 +3566,8 @@
           <t>Bivano per specializzanda</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B126" t="n">
+        <v>0</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3841,10 +3591,8 @@
           <t>Bivano per ragazza specializzanda</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B127" t="n">
+        <v>0</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -3868,10 +3616,8 @@
           <t>Bivano/trivano</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B128" t="n">
+        <v>0</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -3895,10 +3641,8 @@
           <t>Appartamento in viale Poetto</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B129" t="n">
+        <v>0</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -3922,10 +3666,8 @@
           <t>Coppia</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B130" t="n">
+        <v>0</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -3949,10 +3691,8 @@
           <t>Bivano per ragazza lavoratrice</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B131" t="n">
+        <v>0</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3976,10 +3716,8 @@
           <t>60/70mq</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B132" t="n">
+        <v>0</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -4003,10 +3741,8 @@
           <t>Per Piloti/Ass.nti di volo - Appartamento arredato</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B133" t="n">
+        <v>0</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -4030,10 +3766,8 @@
           <t>Appartamento ristrutturato centro</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
+      <c r="B134" t="n">
+        <v>1200</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -4057,10 +3791,8 @@
           <t>Ampio quadrivano</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
+      <c r="B135" t="n">
+        <v>2000</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -4084,10 +3816,8 @@
           <t>Monolocale Cagliari hinterland</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+      <c r="B136" t="n">
+        <v>400</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -4111,10 +3841,8 @@
           <t>Casa max 500</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B137" t="n">
+        <v>500</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -4138,10 +3866,8 @@
           <t>Monolocale in Via Roma a Cagliari</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B138" t="n">
+        <v>500</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -4165,10 +3891,8 @@
           <t>Bilocale 45 centro storico Cagliari</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B139" t="n">
+        <v>500</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -4192,10 +3916,8 @@
           <t>Cagliari Castello piccolo bivano con cortile</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+      <c r="B140" t="n">
+        <v>600</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -4219,10 +3941,8 @@
           <t>Bivano nuovo in centro</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="B141" t="n">
+        <v>650</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -4246,10 +3966,8 @@
           <t>C.e.r.c.o t.r.i.l.o.c.a.l.e</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="B142" t="n">
+        <v>650</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -4273,10 +3991,8 @@
           <t>Bivano pressi via roma</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B143" t="n">
+        <v>700</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
@@ -4300,10 +4016,8 @@
           <t>Quartiere Castello, bilocale arredato</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B144" t="n">
+        <v>700</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
@@ -4327,10 +4041,8 @@
           <t>Elegante monolocale centro storico Cagliari</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B145" t="n">
+        <v>700</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
@@ -4354,10 +4066,8 @@
           <t>Bivano - Cagliari</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B146" t="n">
+        <v>800</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
@@ -4381,10 +4091,8 @@
           <t>Monolocale bilocale appartamento centro cagliari</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>820</t>
-        </is>
+      <c r="B147" t="n">
+        <v>820</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
@@ -4408,10 +4116,8 @@
           <t>Proprietà libera da subito</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B148" t="n">
+        <v>900</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
@@ -4435,10 +4141,8 @@
           <t>Trilocale da 75mt2 in zona San Benedetto</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B149" t="n">
+        <v>900</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
@@ -4462,10 +4166,8 @@
           <t>Apparta</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+      <c r="B150" t="n">
+        <v>900</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
@@ -4489,10 +4191,8 @@
           <t>Trivano in centro Cagliari zona Piazza Yenne</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>920</t>
-        </is>
+      <c r="B151" t="n">
+        <v>920</v>
       </c>
       <c r="C151" t="inlineStr">
         <is>
@@ -4516,10 +4216,8 @@
           <t>Bilocale/trivano</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B152" t="n">
+        <v>0</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
@@ -4543,10 +4241,8 @@
           <t>Appartamento per due due Specializzande</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B153" t="n">
+        <v>0</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -4570,10 +4266,8 @@
           <t>Appartamento studenti universitari</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B154" t="n">
+        <v>0</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -4597,10 +4291,8 @@
           <t>Appartamento o casa indipendente</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B155" t="n">
+        <v>0</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
@@ -4624,10 +4316,8 @@
           <t>Casa da affittare</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B156" t="n">
+        <v>0</v>
       </c>
       <c r="C156" t="inlineStr">
         <is>
@@ -4651,10 +4341,8 @@
           <t>Ultime due camere di quattro a studenti</t>
         </is>
       </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B157" t="n">
+        <v>0</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
@@ -4678,10 +4366,8 @@
           <t>Appartamento quartiere marina</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B158" t="n">
+        <v>0</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -4705,10 +4391,8 @@
           <t>Bilocale rifinito</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B159" t="n">
+        <v>0</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
@@ -4732,10 +4416,8 @@
           <t>POETTO grazioso miniappartamento</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B160" t="n">
+        <v>0</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
@@ -4759,10 +4441,8 @@
           <t>Bilocale/monolocale</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B161" t="n">
+        <v>0</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
@@ -4786,10 +4466,8 @@
           <t>Monolocale / bilocale</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B162" t="n">
+        <v>0</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
@@ -4813,10 +4491,8 @@
           <t>Appartamento arredato bilocale zona S. benedetto</t>
         </is>
       </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B163" t="n">
+        <v>0</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
@@ -4840,10 +4516,8 @@
           <t>Bilocale/monolocale/stanza a Cagliari</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B164" t="n">
+        <v>0</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -4867,10 +4541,8 @@
           <t>Appartamento Centro Storico . Casa vacanze</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B165" t="n">
+        <v>0</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
@@ -4894,10 +4566,8 @@
           <t>Monolocale o bilocale per lavoratrice</t>
         </is>
       </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B166" t="n">
+        <v>0</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -4921,10 +4591,8 @@
           <t>Appartamento con due/tre stanza per 3 studenti</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B167" t="n">
+        <v>0</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
@@ -4948,10 +4616,8 @@
           <t>Appartamenti in Marina</t>
         </is>
       </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>1290</t>
-        </is>
+      <c r="B168" t="n">
+        <v>1290</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
@@ -4975,10 +4641,8 @@
           <t>Appartamento uso ufficio</t>
         </is>
       </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
+      <c r="B169" t="n">
+        <v>3000</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -5002,10 +4666,8 @@
           <t>Coppia referenziata 500</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B170" t="n">
+        <v>500</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
@@ -5029,10 +4691,8 @@
           <t>Centro Storico, Castello Stanze arredate</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="B171" t="n">
+        <v>60</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -5056,10 +4716,8 @@
           <t>Appartamento in via Liguria 1</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+      <c r="B172" t="n">
+        <v>600</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -5083,10 +4741,8 @@
           <t>Casa per coppia referenziata</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+      <c r="B173" t="n">
+        <v>600</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -5110,10 +4766,8 @@
           <t>Luminoso e ampio appartamento Via Is Mirrionis</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+      <c r="B174" t="n">
+        <v>700</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
@@ -5137,10 +4791,8 @@
           <t>Carinissimo appartamento alla Marina</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
+      <c r="B175" t="n">
+        <v>750</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -5164,10 +4816,8 @@
           <t>Monolocali e Bilocali Centro città</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B176" t="n">
+        <v>800</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -5191,10 +4841,8 @@
           <t>Bivano Quartiere del Sole</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
+      <c r="B177" t="n">
+        <v>850</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -6159,6 +5807,970 @@
       <c r="E215" t="inlineStr">
         <is>
           <t>cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2 LOCALI A CAGLIARI</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/2-locali-a-cagliari-cagliari-496745468.htm</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Monolocale Marina centro storico</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-marina-centro-storico-cagliari-496483664.htm</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Bivano arredato zona Piazza Italia</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bivano-arredato-zona-piazza-italia-cagliari-496099079.htm</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Ampio pentavano p.zza Giovanni Cagliari</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>1350</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/ampio-pentavano-p-zza-giovanni-cagliari-cagliari-496014955.htm</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>San Benedetto - appartamento tre camere singole</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/san-benedetto-appartamento-tre-camere-singole-cagliari-495963444.htm</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Maglias ptc</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>580</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/maglias-ptc-cagliari-496125605.htm</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Bilocale via Piero della Francesca 55, Cagliari</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>550</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103752314/</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Appartamento a Cagliari</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>750</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-a-cagliari-cagliari-496411803.htm</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Ampio quadrivano subito disponibile</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>950</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/ampio-quadrivano-subito-disponibile-cagliari-496123486.htm</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Appartamento a Cagliari</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>1100</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-a-cagliari-cagliari-496411793.htm</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Quadrilocale via Giuseppe Manno 49, Castello, Cagliari</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/74437388/</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Via Dante ampio Ttivano piano alto</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/via-dante-ampio-ttivano-piano-alto-cagliari-496535751.htm</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Quadrilocale Pirri</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/quadrilocale-pirri-cagliari-495945390.htm</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Trivano arredato pressi Amsicora</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/trivano-arredato-pressi-amsicora-cagliari-496463795.htm</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Piazza Giovanni XXIII - Rifinito bivano arredato</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/piazza-giovanni-xxiii-rifinito-bivano-arredato-cagliari-495932646.htm</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Stanza</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>270</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/stanza-cagliari-496385665.htm</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Bilocale San Benedetto</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>750</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-san-benedetto-cagliari-495944785.htm</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Bivano - Cagliari</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bivano-cagliari-cagliari-496884505.htm</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Bivano in centro</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bivano-in-centro-cagliari-496607701.htm</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Quadrivano ristrutturato due bagni sauna lavanderi</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/quadrivano-ristrutturato-due-bagni-sauna-lavanderi-cagliari-497001059.htm</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Monolocale via Robert Koch, Monte Claro, Cagliari</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>680</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103671644/</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Bivano Pirri</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bivano-pirri-cagliari-496021719.htm</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Appartamento a Cagliari</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-a-cagliari-cagliari-496411837.htm</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Luminoso quadrivano in via Manno</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/luminoso-quadrivano-in-via-manno-cagliari-495958151.htm</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Nuovissimo Trivano ViaDellaPineta x Medici/Statali</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>1100</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/nuovissimo-trivano-viadellapineta-x-medici-statali-cagliari-496829927.htm</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Piccolo monovano</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/piccolo-monovano-cagliari-496112939.htm</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Prestigioso bivano con ascensore</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/prestigioso-bivano-con-ascensore-cagliari-496959003.htm</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Bivano a Cagliari zona Ospedale Brotzu</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bivano-a-cagliari-zona-ospedale-brotzu-cagliari-496721640.htm</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Stanza uso Ufficio</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/stanza-uso-ufficio-cagliari-496717529.htm</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Genneruxi</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>1100</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/genneruxi-cagliari-496201226.htm</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Appartamento per trasfertisti</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-per-trasfertisti-cagliari-496228738.htm</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Cagliari castello rifinito bivano arredato 50mq</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/cagliari-castello-rifinito-bivano-arredato-50mq-cagliari-496684026.htm</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Ampio quadrivano in via de Martis - Da Agosto</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>1100</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/ampio-quadrivano-in-via-de-martis-da-agosto-cagliari-496359536.htm</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Trilocale via della Pineta 201, Bonaria, Cagliari</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103717220/</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Seminterrato</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/seminterrato-cagliari-496174852.htm</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Cagliari La Vega quadrivano 2 bagni arredato</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/cagliari-la-vega-quadrivano-2-bagni-arredato-cagliari-496439788.htm</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
inserimento ricerca continuativa ogni 30 minuti
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E384"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6716,10 +6716,8 @@
           <t>Trivano arredato via della Pineta</t>
         </is>
       </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+      <c r="B252" t="n">
+        <v>800</v>
       </c>
       <c r="C252" t="inlineStr">
         <is>
@@ -6743,10 +6741,8 @@
           <t>Trilocale nuovo con posto auto da fine giugno</t>
         </is>
       </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>790</t>
-        </is>
+      <c r="B253" t="n">
+        <v>790</v>
       </c>
       <c r="C253" t="inlineStr">
         <is>
@@ -6761,6 +6757,3505 @@
       <c r="E253" t="inlineStr">
         <is>
           <t>cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Quadrilocale via Albert Einstein 13, Cagliari</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103819999/</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Cagliari, via Salvatore Farina, ufficio</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>330</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/cagliari-via-salvatore-farina-ufficio-cagliari-497061466.htm</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Trilocale a Genneruxi</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/trilocale-a-genneruxi-cagliari-497078109.htm</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Via Dante piano alto trivano Luminosissimo</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>850</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/via-dante-piano-alto-trivano-luminosissimo-cagliari-497041749.htm</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>cagliari</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Monolocale arredato abitabile per 1 persona</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-arredato-abitabile-per-1-persona-sassari-488827179.htm</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Monolocale a Sassari</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-a-sassari-sassari-495128439.htm</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Appartamento per studenti</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>750</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-per-studenti-sassari-493337837.htm</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Grazioso monolocale</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/grazioso-monolocale-sassari-496891648.htm</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Viale Umberto Alta</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/viale-umberto-alta-sassari-496065134.htm</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Bilocale via Luigi Rolando 11, Porcellana, Sassari</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>760</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/101621009/</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Appartamento luminosissimo</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-luminosissimo-sassari-490170317.htm</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Via Zanfarino euro 560</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>560</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/via-zanfarino-euro-560-sassari-497096422.htm</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Appartamento Sassari</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-sassari-sassari-495286713.htm</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Bilocale - uso ufficio</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-uso-ufficio-sassari-492255062.htm</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Ufficio in Piazza Castello</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/ufficio-in-piazza-castello-sassari-486825313.htm</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Trilocale - stanze - Via Enrico Costa</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/trilocale-stanze-via-enrico-costa-sassari-493196750.htm</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Monolocale Via IV Novembre</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-via-iv-novembre-sassari-496600123.htm</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Confortevole trilocale</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/confortevole-trilocale-sassari-467554685.htm</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Locale commerciale artigianale attrezzato</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/locale-commerciale-artigianale-attrezzato-sassari-469391139.htm</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Da 1 a 3 mesi bilocale a Sassari</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/da-1-a-3-mesi-bilocale-a-sassari-sassari-475184783.htm</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Appartamentino</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamentino-sassari-453335327.htm</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Trilocale via Damiano Ciancilla 1, Li Punti - Viziliu, Sassari</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>630</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/101817345/</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Bilocale moderno e centrale</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>630</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-moderno-e-centrale-sassari-496916054.htm</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>IN CENTRO rinnovato monolocale arredato</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/in-centro-rinnovato-monolocale-arredato-sassari-494897445.htm</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Appartamento o villa</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-o-villa-sassari-496170488.htm</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Quadrilocale Li Punti centralissimo</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/quadrilocale-li-punti-centralissimo-sassari-449104776.htm</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Appartamento ristrutturato</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-ristrutturato-sassari-462566779.htm</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Ricerco coinquilina</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/ricerco-coinquilina-sassari-497007411.htm</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Grazioso bilocale pressi Via Brigata Sassari</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>420</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/grazioso-bilocale-pressi-via-brigata-sassari-sassari-496353382.htm</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Monolocale via al Duomo 1A, Centro Storico, Sassari</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>290</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103121958/</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Affitti</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/affitti-sassari-487592167.htm</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Appartamento per giovane coppia</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-per-giovane-coppia-sassari-496931985.htm</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Appartamento in villa trifamiliare</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-in-villa-trifamiliare-sassari-496615667.htm</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Camera in appartamento a Sassari</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/camera-in-appartamento-a-sassari-sassari-465327504.htm</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Bilocale pressi via Napoli</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-pressi-via-napoli-sassari-496624543.htm</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Appartamento via Umana, 15, Carbonazzi - Acquedotto, Sassari</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>650</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103643394/</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Bilocale zona via alghero</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-zona-via-alghero-sassari-466941361.htm</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Stanze per studenti</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>387</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/stanze-per-studenti-sassari-474705443.htm</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Appartamento arredato</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-arredato-sassari-480994254.htm</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Attico in centro per brevi periodi</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/attico-in-centro-per-brevi-periodi-sassari-463860670.htm</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Monolocale viale Adua, Luna e Sole - Prunizzedda, Sassari</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>480</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/102233908/</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Studio pressi Ospedali al piano terra</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/studio-pressi-ospedali-al-piano-terra-sassari-495322420.htm</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Monolocale Santa Teresa Gallura</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-santa-teresa-gallura-sassari-496542247.htm</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Massima urgenza un appartamento</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/massima-urgenza-un-appartamento-sassari-478711991.htm</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Bi-tri locale</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bi-tri-locale-sassari-456539901.htm</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Appartamento a Sassari</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-a-sassari-sassari-471495889.htm</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Casa a Sassari</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-a-sassari-sassari-463544239.htm</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Casa per giovane coppia</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-per-giovane-coppia-sassari-466028260.htm</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Locale per 1 o 2 persone</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/locale-per-1-o-2-persone-sassari-495356946.htm</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Appartamento Alghero</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-alghero-sassari-479571847.htm</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Appartamento arredato Li Punti</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-arredato-li-punti-sassari-494389966.htm</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Quadrilocale via rockfeller 19, Porcellana, Sassari</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>170</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/98941950/</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Appartamento vicino Ospedali/Università</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-vicino-ospedali-universita-sassari-489855679.htm</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Alloggio platamona</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/alloggio-platamona-sassari-455623481.htm</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Una casa contratto mensile</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/una-casa-contratto-mensile-sassari-488412894.htm</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Bilocale per Studenti e trasfertisti</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-per-studenti-e-trasfertisti-sassari-493820864.htm</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Casa condivisa camera singola in appartamento</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-condivisa-camera-singola-in-appartamento-sassari-496969744.htm</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Appartamento pressi ospedale Sassari</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-pressi-ospedale-sassari-sassari-483754674.htm</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Appartamento Via Matteotti Sassari</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-via-matteotti-sassari-sassari-491924914.htm</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Bilocale arredato pressi cliniche San Pietro</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-arredato-pressi-cliniche-san-pietro-sassari-497063787.htm</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>L'appartamento per una brava ragazza</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/l-appartamento-per-una-brava-ragazza-sassari-496950712.htm</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Zona Ospedale Civile - Via Monte Grappa</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/zona-ospedale-civile-via-monte-grappa-sassari-493521715.htm</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Trilocale via biasi, 7 a, Luna e Sole - Prunizzedda, Sassari</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>600</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103375496/</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Appartamento libero</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-libero-sassari-496998444.htm</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Sassari centro presso il museo</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/sassari-centro-presso-il-museo-sassari-452218469.htm</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>3 LOCALI A SASSARI</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>630</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/3-locali-a-sassari-sassari-491966174.htm</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Monolocale via Università,pressi p.zza Azuni</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>360</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-via-universita-pressi-p-zza-azuni-sassari-495884802.htm</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Monti bianchinu</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>420</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monti-bianchinu-sassari-465112764.htm</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Bivano arredato</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>430</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bivano-arredato-sassari-496950186.htm</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Ampio luminoso monolocale</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/ampio-luminoso-monolocale-sassari-488964077.htm</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/sassari-sassari-479728833.htm</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Mansarda altezza abitabile</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/mansarda-altezza-abitabile-sassari-459438630.htm</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Appartamento in via Catalocchino arredato</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>1050</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-in-via-catalocchino-arredato-sassari-494762675.htm</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Appartamento corso Giovanni Maria Angioj, Porcellana, Sassari</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>600</v>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/95835948/</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Luminoso bilocale zona S.Orsola-SS</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/luminoso-bilocale-zona-s-orsola-ss-sassari-494471853.htm</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Rtl124</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/rtl124-sassari-480366546.htm</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Studenti/ lavoratori zona ospedale</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/studenti-lavoratori-zona-ospedale-sassari-494555209.htm</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Appartamento a Sassari</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-a-sassari-sassari-465978998.htm</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Via p.paoli in palazzina d'epoca euro 700</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/via-p-paoli-in-palazzina-d-epoca-euro-700-sassari-490234968.htm</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>PIAZZA AZUNI interessante locale commerciale</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/piazza-azuni-interessante-locale-commerciale-sassari-444239753.htm</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Appartamento piazza Castello, Centro Storico, Sassari</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>700</v>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103669828/</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Appartamento arredato</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-arredato-sassari-494566782.htm</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Adiacenze Viale UMBERTO</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/adiacenze-viale-umberto-sassari-472415192.htm</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Villa unifamiliare via Argentiera, Palmadula - Argentiera, Sassari</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/102160090/</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Monolocale via P Maria angolo viale Italia</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-via-p-maria-angolo-viale-italia-sassari-496250271.htm</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Bilocale ristrutturato</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-ristrutturato-sassari-482874243.htm</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Monolocale Cugnana/Olbia</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-cugnana-olbia-sassari-460136604.htm</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>Monolocali Piazza Azuni</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocali-piazza-azuni-sassari-495941866.htm</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Santa Teresa Gallura Capotesta</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/santa-teresa-gallura-capotesta-sassari-497061342.htm</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Appartamento arredato</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-arredato-sassari-465935222.htm</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/sassari-sassari-491540696.htm</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>Trilocale non arredato</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/trilocale-non-arredato-sassari-480388816.htm</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>In afito</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/in-afito-sassari-459690086.htm</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>Sassari immobile</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/sassari-immobile-sassari-479906428.htm</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>Trilocale uso studio Piazza Fiume</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/trilocale-uso-studio-piazza-fiume-sassari-496458347.htm</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>Bilocale/trilocale</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-trilocale-sassari-483580843.htm</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>Monolocale Sassari Centrale</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-sassari-centrale-sassari-492551697.htm</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>Appartamenti in villa senza spese condominiali</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamenti-in-villa-senza-spese-condominiali-sassari-496275005.htm</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>Bilocale Vico Vincenzo Sulis 3, Centro Storico, Sassari</t>
+        </is>
+      </c>
+      <c r="B352" t="n">
+        <v>350</v>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103312958/</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>Bilocale via Roma Sassari</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-via-roma-sassari-sassari-496814018.htm</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>Appartamento non arredato</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-non-arredato-sassari-472081738.htm</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>Appartamento studenti via Sardegna Sassari</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-studenti-via-sardegna-sassari-sassari-450701423.htm</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Quadrilocale via parigi 2, Rizzeddu - Monserrato, Sassari</t>
+        </is>
+      </c>
+      <c r="B356" t="n">
+        <v>230</v>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/103834697/</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>Bi/trilocale per una famiglia di tre persone</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bi-trilocale-per-una-famiglia-di-tre-persone-sassari-487926277.htm</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Appartamento in campagna</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-in-campagna-sassari-476046865.htm</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Casa per trasfertista</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-per-trasfertista-sassari-496646781.htm</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Stanze</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/stanze-sassari-456865561.htm</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>Bilocale via Giovanni Amendola 72, Porcellana, Sassari</t>
+        </is>
+      </c>
+      <c r="B361" t="n">
+        <v>620</v>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/101593859/</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>Appartamento in città o in campagna</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-in-citta-o-in-campagna-sassari-452712732.htm</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Quadrilocale via Carlo Alberto 12, Centro Storico, Sassari</t>
+        </is>
+      </c>
+      <c r="B363" t="n">
+        <v>280</v>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/100482346/</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Appartamento zona Sassari, Li Punti o Usini</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-zona-sassari-li-punti-o-usini-sassari-489145319.htm</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Stanze</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/stanze-sassari-461467346.htm</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>Appartamento per coppia</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-per-coppia-sassari-494286482.htm</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>Bilocale via Aldo Cesaraccio 39, Sant'Orsola, Sassari</t>
+        </is>
+      </c>
+      <c r="B367" t="n">
+        <v>600</v>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.immobiliare.it/annunci/82367632/</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Appartamento bi/trilocale</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-bi-trilocale-sassari-492100286.htm</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Affitti</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/affitti-sassari-486854434.htm</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Monolocale interamente ristrutturato</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>430</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-interamente-ristrutturato-sassari-449040475.htm</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Bilocale 3 piano luminoso e silenzioso</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>460</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-3-piano-luminoso-e-silenzioso-sassari-496263691.htm</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Bilocale via Risorgimento 59 Sassari</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-via-risorgimento-59-sassari-sassari-495924338.htm</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Trilocale Sassari</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/trilocale-sassari-sassari-461087420.htm</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Monolocale bilocale</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/monolocale-bilocale-sassari-484647988.htm</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Casa in periferia</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-in-periferia-sassari-453487766.htm</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>Bilocale arredato</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-arredato-sassari-495876207.htm</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>Bilocale-recente costruzione - Via Nurra -Sassari</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/bilocale-recente-costruzione-via-nurra-sassari-sassari-491789846.htm</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>VIA POLA angolo VIA GORIZIA</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/via-pola-angolo-via-gorizia-sassari-490525957.htm</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Camere singole</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/camere-singole-sassari-457874790.htm</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Casa o appartamento con contratto mensile</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-o-appartamento-con-contratto-mensile-sassari-484376525.htm</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Casa in Corso Trinità</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/casa-in-corso-trinita-sassari-457391497.htm</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Appartamento Sassari città</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-sassari-citta-sassari-457756706.htm</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Appartamento in villa in campagna</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-in-villa-in-campagna-sassari-495727108.htm</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>Sassari</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Appartamento per coppia con un bimbo</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.subito.it/appartamenti/appartamento-per-coppia-con-un-bimbo-sassari-480186405.htm</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>No_Data</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>Sassari</t>
         </is>
       </c>
     </row>

</xml_diff>